<commit_message>
correction stage 3 evidence for B1 + B5,B6,B7 tasks
</commit_message>
<xml_diff>
--- a/furkanefe-oss/evidence.xlsx
+++ b/furkanefe-oss/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frkn_\Desktop\gon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA843FA5-7B50-4EBC-9951-EEBF9A3E22CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200D78FA-65C9-41C1-AD97-E55F8F0DB2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="924" windowWidth="17280" windowHeight="10008" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="1224" windowWidth="16560" windowHeight="10008" firstSheet="14" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="103">
   <si>
     <t>TxHash</t>
   </si>
@@ -329,6 +330,30 @@
   </si>
   <si>
     <t>3148AD22604271D4F98B03C9E613BB01411C9BD6EE8EE050CE2624F6CC240B7C</t>
+  </si>
+  <si>
+    <t>4B6EE9A41A4F055D5642AA796576087EA60B069EA88A75321F245A65F6046418</t>
+  </si>
+  <si>
+    <t>50B91747D02C2CBFD97557733BDA493465167B2D30D2598E0C97614CA2B566B4</t>
+  </si>
+  <si>
+    <t>4F30A00BCD77AC383713D2449D94F48FC23F79FC679036DFD27B104B5294798F</t>
+  </si>
+  <si>
+    <t>959A861D08670153E84D8F7D4412756AE9E1488B95C881AD6A7F7214C7386869</t>
+  </si>
+  <si>
+    <t>CDB428A555B115D05ED72038D3AEC7D496F50CDD8F20FE292998AC481B07E866</t>
+  </si>
+  <si>
+    <t>E03910F29DAB97D8C32E9CA1E0FBA522AA67C38F33CDE0B7FF7A3F8C98E4E364</t>
+  </si>
+  <si>
+    <t>9B139418B837ADB23F7056ADF9ADEFA6BE7C30053D3D63B6693EB4176EB80638</t>
+  </si>
+  <si>
+    <t>F2D8BB8E9EB930C0E46C330C9C8E4DE3BCE89D7AAC22B606D0EC6EFF0204696F</t>
   </si>
 </sst>
 </file>
@@ -457,7 +482,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -465,15 +490,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,70 +506,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="8" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="11" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="12" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="11" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="14" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="15" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="16" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="16" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="18" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="19" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="20" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="18" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="19" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="20" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="21" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="22" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="23" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="24" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="22" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="23" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="24" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="26" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="27" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="28" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="29" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="30" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="27" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="28" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="29" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="30" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="31" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="32" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="33" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="34" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="35" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="31" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="32" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="33" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="34" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="35" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="36" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="37" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="38" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="39" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="40" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="41" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="37" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="39" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="40" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="41" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -899,19 +922,19 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -941,28 +964,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -984,8 +1007,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1022,8 +1045,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1060,8 +1083,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1098,8 +1121,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1136,8 +1159,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1152,7 +1175,7 @@
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1160,7 +1183,7 @@
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1168,15 +1191,15 @@
       <c r="A4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1199,8 +1222,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1215,7 +1238,7 @@
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1223,7 +1246,7 @@
       <c r="A3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1231,15 +1254,15 @@
       <c r="A4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1261,8 +1284,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1277,7 +1300,7 @@
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1285,7 +1308,7 @@
       <c r="A3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1293,15 +1316,15 @@
       <c r="A4" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1323,8 +1346,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1339,7 +1362,7 @@
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1347,7 +1370,7 @@
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1355,15 +1378,15 @@
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="27" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1385,8 +1408,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1401,7 +1424,7 @@
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1409,7 +1432,7 @@
       <c r="A3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1417,15 +1440,15 @@
       <c r="A4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1447,8 +1470,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1463,7 +1486,7 @@
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="33" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1471,7 +1494,7 @@
       <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1479,15 +1502,15 @@
       <c r="A4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="36" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1509,7 +1532,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1546,8 +1569,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1562,7 +1585,7 @@
       <c r="A2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1570,7 +1593,7 @@
       <c r="A3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="38" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1578,31 +1601,31 @@
       <c r="A4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="41" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="42" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1624,8 +1647,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1640,7 +1663,7 @@
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1648,39 +1671,39 @@
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="45" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="47" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="48" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1694,13 +1717,59 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1708,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1723,18 +1792,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1744,31 +1815,33 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1778,46 +1851,45 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85ABBBF9-4CA2-4974-A8C1-D40F55D9D6D6}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1832,14 +1904,14 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1857,73 +1929,73 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1944,9 +2016,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1973,6 +2045,108 @@
       <c r="C2" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="D2" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="D2" s="11" t="s">
         <v>34</v>
       </c>
@@ -1982,12 +2156,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1995,162 +2259,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2163,44 +2273,6 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">

</xml_diff>